<commit_message>
Added VAT valve to drawing. Millions of parts changed for no good reason.
</commit_message>
<xml_diff>
--- a/8020 enclosure rev2/enclosure rev2 parts list.xlsx
+++ b/8020 enclosure rev2/enclosure rev2 parts list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Line #</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>7155 Cut to size 7.86 x 53 inches</t>
+  </si>
+  <si>
+    <t>lower long</t>
+  </si>
+  <si>
+    <t>7010 cut to length. 7040 sides A and C, both ends.</t>
   </si>
 </sst>
 </file>
@@ -471,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:H17"/>
+  <dimension ref="B4:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,6 +787,29 @@
       </c>
       <c r="H17" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>1515</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>48.19</v>
+      </c>
+      <c r="H18" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected error in panel sizing.
</commit_message>
<xml_diff>
--- a/8020 enclosure rev2/enclosure rev2 parts list.xlsx
+++ b/8020 enclosure rev2/enclosure rev2 parts list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Line #</t>
   </si>
@@ -132,12 +132,24 @@
   <si>
     <t>7010 cut to length. 7040 sides A and C, both ends.</t>
   </si>
+  <si>
+    <t>I made a size error</t>
+  </si>
+  <si>
+    <t>Replacement order for panels</t>
+  </si>
+  <si>
+    <t>7155 Cut to size 9.86 x 53 inches</t>
+  </si>
+  <si>
+    <t>7155 Cut to size 10.98 x 53 inches</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,13 +165,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -171,13 +195,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -477,10 +504,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:H18"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B4:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +521,7 @@
     <col min="8" max="8" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -514,7 +544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -537,7 +567,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2</v>
       </c>
@@ -560,7 +590,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>3</v>
       </c>
@@ -574,7 +604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>4</v>
       </c>
@@ -588,7 +618,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>5</v>
       </c>
@@ -611,7 +641,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>6</v>
       </c>
@@ -634,7 +664,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>7</v>
       </c>
@@ -657,7 +687,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>8</v>
       </c>
@@ -680,7 +710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>9</v>
       </c>
@@ -703,7 +733,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>10</v>
       </c>
@@ -726,7 +756,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>11</v>
       </c>
@@ -749,47 +779,55 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
         <v>12</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>2610</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>8</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H16" t="s">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="I16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
         <v>13</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>2610</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>8</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H17" t="s">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>14</v>
       </c>
@@ -812,9 +850,54 @@
         <v>33</v>
       </c>
     </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>2610</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>2610</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="61" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>